<commit_message>
final refinements, update documentation
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjornnelson/SimplicityStudio/v5_workspace/ecen5823-assignment6-bjornhnelson/questions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjornnelson/SimplicityStudio/v5_workspace/ecen5823-assignment7-bjornhnelson/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87F8D28-5638-0F4D-A3AA-BD14DDE804B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5B0EAC-64D8-AB4F-9F9E-6485E9369B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -295,6 +295,18 @@
   </si>
   <si>
     <t>Pass in saved address and address type parameters</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION - handling indications</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION - connected, DISPLAY_ROW_BTADDR2 - server address</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_TEMPVALUE - temp value</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION - discovering, DISPLAY_ROW_NAME - client, DISPLAY_ROW_BTADDR - client address, DISPLAY_ROW_ASSIGNMENT - A7</t>
   </si>
 </sst>
 </file>
@@ -1808,8 +1820,8 @@
   </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="116" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1918,7 +1930,9 @@
       <c r="C7" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="29" t="s">
+        <v>76</v>
+      </c>
       <c r="E7" s="29" t="s">
         <v>56</v>
       </c>
@@ -2010,7 +2024,9 @@
       <c r="C13" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="29" t="s">
+        <v>74</v>
+      </c>
       <c r="E13" s="24" t="s">
         <v>46</v>
       </c>
@@ -2240,7 +2256,9 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="16"/>
+      <c r="D29" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="24" t="s">
@@ -2336,7 +2354,9 @@
       <c r="C36" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="E36" s="16" t="s">
         <v>56</v>
       </c>

</xml_diff>